<commit_message>
adding category on asset seed
</commit_message>
<xml_diff>
--- a/stadia/seed/computer_and_acc.xlsx
+++ b/stadia/seed/computer_and_acc.xlsx
@@ -2135,11 +2135,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L115" activeCellId="0" sqref="L115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A42" colorId="64" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M44" activeCellId="0" sqref="M44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.57"/>
@@ -2163,7 +2163,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="true" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="17" customFormat="true" ht="49.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="M47" s="37" t="n">
         <f aca="false">J47-K47-L47</f>
-        <v>4441.86881545455</v>
+        <v>4441.86881545457</v>
       </c>
       <c r="N47" s="41"/>
       <c r="O47" s="26"/>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="M50" s="37" t="n">
         <f aca="false">J50-K50-L50</f>
-        <v>979.130826666667</v>
+        <v>979.130826666704</v>
       </c>
       <c r="N50" s="41"/>
       <c r="O50" s="26"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="M51" s="37" t="n">
         <f aca="false">J51-K51-L51</f>
-        <v>219.165796666666</v>
+        <v>219.165796666699</v>
       </c>
       <c r="N51" s="41"/>
       <c r="O51" s="26"/>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="M56" s="37" t="n">
         <f aca="false">J56-K56-L56</f>
-        <v>1410.12943545454</v>
+        <v>1410.12943545457</v>
       </c>
       <c r="N56" s="41"/>
       <c r="O56" s="26"/>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="M58" s="37" t="n">
         <f aca="false">J58-K58-L58</f>
-        <v>3594.86767142857</v>
+        <v>3594.8676714286</v>
       </c>
       <c r="N58" s="41"/>
       <c r="O58" s="26"/>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="M63" s="37" t="n">
         <f aca="false">J63-K63-L63</f>
-        <v>221.470225454548</v>
+        <v>221.470225454603</v>
       </c>
       <c r="N63" s="41"/>
       <c r="O63" s="26"/>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="M69" s="37" t="n">
         <f aca="false">J69-K69-L69</f>
-        <v>1410.12943545454</v>
+        <v>1410.12943545457</v>
       </c>
       <c r="N69" s="41"/>
       <c r="O69" s="26"/>
@@ -5579,7 +5579,7 @@
       </c>
       <c r="M72" s="37" t="n">
         <f aca="false">J72-K72-L72</f>
-        <v>4755.79676545454</v>
+        <v>4755.79676545457</v>
       </c>
       <c r="N72" s="41"/>
       <c r="O72" s="26"/>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="M81" s="37" t="n">
         <f aca="false">J81-K81-L81</f>
-        <v>3544.02548142857</v>
+        <v>3544.0254814286</v>
       </c>
       <c r="N81" s="66"/>
       <c r="O81" s="26"/>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="M83" s="37" t="n">
         <f aca="false">J83-K83-L83</f>
-        <v>4755.79676545454</v>
+        <v>4755.79676545457</v>
       </c>
       <c r="N83" s="41"/>
       <c r="O83" s="26"/>
@@ -6813,14 +6813,15 @@
       <c r="J98" s="77" t="n">
         <v>14956.52</v>
       </c>
-      <c r="K98" s="36" t="e">
-        <f aca="false">#REF!*I98*J98</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L98" s="77"/>
-      <c r="M98" s="37" t="e">
+      <c r="K98" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" s="37" t="n">
         <f aca="false">J98-K98-L98</f>
-        <v>#REF!</v>
+        <v>14956.52</v>
       </c>
       <c r="N98" s="78" t="s">
         <v>375</v>
@@ -6860,14 +6861,15 @@
       <c r="J99" s="77" t="n">
         <v>35217.39</v>
       </c>
-      <c r="K99" s="36" t="e">
-        <f aca="false">#REF!*I99*J99</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L99" s="77"/>
-      <c r="M99" s="37" t="e">
+      <c r="K99" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" s="37" t="n">
         <f aca="false">J99-K99-L99</f>
-        <v>#REF!</v>
+        <v>35217.39</v>
       </c>
       <c r="N99" s="78" t="s">
         <v>375</v>
@@ -6907,14 +6909,15 @@
       <c r="J100" s="77" t="n">
         <v>35217.39</v>
       </c>
-      <c r="K100" s="36" t="e">
-        <f aca="false">#REF!*I100*J100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L100" s="77"/>
-      <c r="M100" s="37" t="e">
+      <c r="K100" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" s="37" t="n">
         <f aca="false">J100-K100-L100</f>
-        <v>#REF!</v>
+        <v>35217.39</v>
       </c>
       <c r="N100" s="78" t="s">
         <v>375</v>
@@ -6954,14 +6957,15 @@
       <c r="J101" s="81" t="n">
         <v>6869.56</v>
       </c>
-      <c r="K101" s="36" t="e">
-        <f aca="false">#REF!*I101*J101</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L101" s="37"/>
-      <c r="M101" s="37" t="e">
+      <c r="K101" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" s="37" t="n">
         <f aca="false">J101-K101-L101</f>
-        <v>#REF!</v>
+        <v>6869.56</v>
       </c>
       <c r="N101" s="78" t="s">
         <v>375</v>
@@ -6996,14 +7000,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K102" s="36" t="e">
-        <f aca="false">#REF!*I102*J102</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L102" s="36"/>
-      <c r="M102" s="37" t="e">
+      <c r="K102" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" s="37" t="n">
         <f aca="false">J102-K102-L102</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N102" s="78" t="s">
         <v>375</v>
@@ -7038,14 +7043,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K103" s="36" t="e">
-        <f aca="false">#REF!*I103*J103</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L103" s="36"/>
-      <c r="M103" s="37" t="e">
+      <c r="K103" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" s="37" t="n">
         <f aca="false">J103-K103-L103</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N103" s="78" t="s">
         <v>375</v>
@@ -7080,14 +7086,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K104" s="36" t="e">
-        <f aca="false">#REF!*I104*J104</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L104" s="36"/>
-      <c r="M104" s="37" t="e">
+      <c r="K104" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" s="37" t="n">
         <f aca="false">J104-K104-L104</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N104" s="78" t="s">
         <v>375</v>
@@ -7122,14 +7129,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K105" s="36" t="e">
-        <f aca="false">#REF!*I105*J105</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L105" s="36"/>
-      <c r="M105" s="37" t="e">
+      <c r="K105" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" s="37" t="n">
         <f aca="false">J105-K105-L105</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N105" s="78" t="s">
         <v>375</v>
@@ -7164,14 +7172,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K106" s="36" t="e">
-        <f aca="false">#REF!*I106*J106</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L106" s="36"/>
-      <c r="M106" s="37" t="e">
+      <c r="K106" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" s="37" t="n">
         <f aca="false">J106-K106-L106</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N106" s="78" t="s">
         <v>375</v>
@@ -7206,14 +7215,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K107" s="36" t="e">
-        <f aca="false">#REF!*I107*J107</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L107" s="36"/>
-      <c r="M107" s="37" t="e">
+      <c r="K107" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L107" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" s="37" t="n">
         <f aca="false">J107-K107-L107</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N107" s="78" t="s">
         <v>375</v>
@@ -7248,14 +7258,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K108" s="36" t="e">
-        <f aca="false">#REF!*I108*J108</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L108" s="36"/>
-      <c r="M108" s="37" t="e">
+      <c r="K108" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" s="37" t="n">
         <f aca="false">J108-K108-L108</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N108" s="78" t="s">
         <v>375</v>
@@ -7290,14 +7301,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K109" s="36" t="e">
-        <f aca="false">#REF!*I109*J109</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L109" s="36"/>
-      <c r="M109" s="37" t="e">
+      <c r="K109" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L109" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" s="37" t="n">
         <f aca="false">J109-K109-L109</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N109" s="78" t="s">
         <v>375</v>
@@ -7332,14 +7344,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K110" s="36" t="e">
-        <f aca="false">#REF!*I110*J110</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L110" s="36"/>
-      <c r="M110" s="37" t="e">
+      <c r="K110" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" s="37" t="n">
         <f aca="false">J110-K110-L110</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N110" s="78" t="s">
         <v>375</v>
@@ -7374,14 +7387,15 @@
         <f aca="false">16500</f>
         <v>16500</v>
       </c>
-      <c r="K111" s="36" t="e">
-        <f aca="false">#REF!*I111*J111</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L111" s="36"/>
-      <c r="M111" s="37" t="e">
+      <c r="K111" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" s="37" t="n">
         <f aca="false">J111-K111-L111</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N111" s="78" t="s">
         <v>375</v>
@@ -7416,14 +7430,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K112" s="36" t="e">
-        <f aca="false">#REF!*I112*J112</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L112" s="36"/>
-      <c r="M112" s="37" t="e">
+      <c r="K112" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L112" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M112" s="37" t="n">
         <f aca="false">J112-K112-L112</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N112" s="78" t="s">
         <v>375</v>
@@ -7458,14 +7473,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K113" s="36" t="e">
-        <f aca="false">#REF!*I113*J113</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L113" s="36"/>
-      <c r="M113" s="37" t="e">
+      <c r="K113" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L113" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" s="37" t="n">
         <f aca="false">J113-K113-L113</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N113" s="78" t="s">
         <v>375</v>
@@ -7500,14 +7516,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K114" s="36" t="e">
-        <f aca="false">#REF!*I114*J114</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L114" s="36"/>
-      <c r="M114" s="37" t="e">
+      <c r="K114" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" s="37" t="n">
         <f aca="false">J114-K114-L114</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N114" s="78" t="s">
         <v>375</v>
@@ -7542,14 +7559,15 @@
         <f aca="false">16000</f>
         <v>16000</v>
       </c>
-      <c r="K115" s="36" t="e">
-        <f aca="false">#REF!*I115*J115</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L115" s="36"/>
-      <c r="M115" s="37" t="e">
+      <c r="K115" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L115" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M115" s="37" t="n">
         <f aca="false">J115-K115-L115</f>
-        <v>#REF!</v>
+        <v>16000</v>
       </c>
       <c r="N115" s="78" t="s">
         <v>375</v>
@@ -7584,14 +7602,15 @@
         <f aca="false">16000</f>
         <v>16000</v>
       </c>
-      <c r="K116" s="36" t="e">
-        <f aca="false">#REF!*I116*J116</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L116" s="36"/>
-      <c r="M116" s="37" t="e">
+      <c r="K116" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L116" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" s="37" t="n">
         <f aca="false">J116-K116-L116</f>
-        <v>#REF!</v>
+        <v>16000</v>
       </c>
       <c r="N116" s="78" t="s">
         <v>375</v>
@@ -7626,14 +7645,15 @@
         <f aca="false">12000</f>
         <v>12000</v>
       </c>
-      <c r="K117" s="36" t="e">
-        <f aca="false">#REF!*I117*J117</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L117" s="36"/>
-      <c r="M117" s="37" t="e">
+      <c r="K117" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" s="37" t="n">
         <f aca="false">J117-K117-L117</f>
-        <v>#REF!</v>
+        <v>12000</v>
       </c>
       <c r="N117" s="78" t="s">
         <v>375</v>
@@ -7668,14 +7688,15 @@
         <f aca="false">12000</f>
         <v>12000</v>
       </c>
-      <c r="K118" s="36" t="e">
-        <f aca="false">#REF!*I118*J118</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L118" s="36"/>
-      <c r="M118" s="37" t="e">
+      <c r="K118" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" s="37" t="n">
         <f aca="false">J118-K118-L118</f>
-        <v>#REF!</v>
+        <v>12000</v>
       </c>
       <c r="N118" s="78" t="s">
         <v>375</v>
@@ -7710,14 +7731,15 @@
         <f aca="false">31304.35</f>
         <v>31304.35</v>
       </c>
-      <c r="K119" s="36" t="e">
-        <f aca="false">#REF!*I119*J119</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L119" s="36"/>
-      <c r="M119" s="37" t="e">
+      <c r="K119" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" s="37" t="n">
         <f aca="false">J119-K119-L119</f>
-        <v>#REF!</v>
+        <v>31304.35</v>
       </c>
       <c r="N119" s="78" t="s">
         <v>375</v>
@@ -7752,14 +7774,15 @@
         <f aca="false">31304.35</f>
         <v>31304.35</v>
       </c>
-      <c r="K120" s="36" t="e">
-        <f aca="false">#REF!*I120*J120</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L120" s="36"/>
-      <c r="M120" s="37" t="e">
+      <c r="K120" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L120" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" s="37" t="n">
         <f aca="false">J120-K120-L120</f>
-        <v>#REF!</v>
+        <v>31304.35</v>
       </c>
       <c r="N120" s="78" t="s">
         <v>375</v>
@@ -7793,14 +7816,15 @@
       <c r="J121" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K121" s="36" t="e">
-        <f aca="false">#REF!*I121*J121</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L121" s="36"/>
-      <c r="M121" s="37" t="e">
+      <c r="K121" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L121" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" s="37" t="n">
         <f aca="false">J121-K121-L121</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N121" s="78" t="s">
         <v>375</v>
@@ -7834,14 +7858,15 @@
       <c r="J122" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K122" s="36" t="e">
-        <f aca="false">#REF!*I122*J122</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L122" s="36"/>
-      <c r="M122" s="37" t="e">
+      <c r="K122" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" s="37" t="n">
         <f aca="false">J122-K122-L122</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N122" s="78" t="s">
         <v>375</v>
@@ -7875,14 +7900,15 @@
       <c r="J123" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K123" s="36" t="e">
-        <f aca="false">#REF!*I123*J123</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L123" s="36"/>
-      <c r="M123" s="37" t="e">
+      <c r="K123" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L123" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" s="37" t="n">
         <f aca="false">J123-K123-L123</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N123" s="78" t="s">
         <v>375</v>
@@ -7916,14 +7942,15 @@
       <c r="J124" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K124" s="36" t="e">
-        <f aca="false">#REF!*I124*J124</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L124" s="36"/>
-      <c r="M124" s="37" t="e">
+      <c r="K124" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" s="37" t="n">
         <f aca="false">J124-K124-L124</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N124" s="78" t="s">
         <v>375</v>
@@ -7957,14 +7984,15 @@
       <c r="J125" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K125" s="36" t="e">
-        <f aca="false">#REF!*I125*J125</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L125" s="36"/>
-      <c r="M125" s="37" t="e">
+      <c r="K125" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M125" s="37" t="n">
         <f aca="false">J125-K125-L125</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N125" s="78" t="s">
         <v>375</v>
@@ -7998,14 +8026,15 @@
       <c r="J126" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K126" s="36" t="e">
-        <f aca="false">#REF!*I126*J126</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L126" s="36"/>
-      <c r="M126" s="37" t="e">
+      <c r="K126" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L126" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M126" s="37" t="n">
         <f aca="false">J126-K126-L126</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N126" s="78" t="s">
         <v>375</v>
@@ -8039,14 +8068,15 @@
       <c r="J127" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K127" s="36" t="e">
-        <f aca="false">#REF!*I127*J127</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L127" s="36"/>
-      <c r="M127" s="37" t="e">
+      <c r="K127" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" s="37" t="n">
         <f aca="false">J127-K127-L127</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N127" s="78" t="s">
         <v>375</v>
@@ -8080,14 +8110,15 @@
       <c r="J128" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K128" s="36" t="e">
-        <f aca="false">#REF!*I128*J128</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L128" s="36"/>
-      <c r="M128" s="37" t="e">
+      <c r="K128" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" s="37" t="n">
         <f aca="false">J128-K128-L128</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N128" s="78" t="s">
         <v>375</v>
@@ -8121,14 +8152,15 @@
       <c r="J129" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K129" s="36" t="e">
-        <f aca="false">#REF!*I129*J129</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L129" s="36"/>
-      <c r="M129" s="37" t="e">
+      <c r="K129" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" s="37" t="n">
         <f aca="false">J129-K129-L129</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N129" s="78" t="s">
         <v>375</v>
@@ -8162,14 +8194,15 @@
       <c r="J130" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K130" s="36" t="e">
-        <f aca="false">#REF!*I130*J130</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L130" s="36"/>
-      <c r="M130" s="37" t="e">
+      <c r="K130" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" s="37" t="n">
         <f aca="false">J130-K130-L130</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N130" s="78" t="s">
         <v>375</v>
@@ -8203,14 +8236,15 @@
       <c r="J131" s="81" t="n">
         <v>16500</v>
       </c>
-      <c r="K131" s="36" t="e">
-        <f aca="false">#REF!*I131*J131</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L131" s="36"/>
-      <c r="M131" s="37" t="e">
+      <c r="K131" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" s="37" t="n">
         <f aca="false">J131-K131-L131</f>
-        <v>#REF!</v>
+        <v>16500</v>
       </c>
       <c r="N131" s="78" t="s">
         <v>375</v>
@@ -8245,14 +8279,15 @@
         <f aca="false">13000</f>
         <v>13000</v>
       </c>
-      <c r="K132" s="36" t="e">
-        <f aca="false">#REF!*I132*J132</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L132" s="36"/>
-      <c r="M132" s="37" t="e">
+      <c r="K132" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" s="37" t="n">
         <f aca="false">J132-K132-L132</f>
-        <v>#REF!</v>
+        <v>13000</v>
       </c>
       <c r="N132" s="78" t="s">
         <v>375</v>
@@ -8287,14 +8322,15 @@
         <f aca="false">13000</f>
         <v>13000</v>
       </c>
-      <c r="K133" s="36" t="e">
-        <f aca="false">#REF!*I133*J133</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L133" s="36"/>
-      <c r="M133" s="37" t="e">
+      <c r="K133" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" s="37" t="n">
         <f aca="false">J133-K133-L133</f>
-        <v>#REF!</v>
+        <v>13000</v>
       </c>
       <c r="N133" s="78" t="s">
         <v>375</v>
@@ -8329,14 +8365,15 @@
         <f aca="false">13000</f>
         <v>13000</v>
       </c>
-      <c r="K134" s="36" t="e">
-        <f aca="false">#REF!*I134*J134</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L134" s="36"/>
-      <c r="M134" s="37" t="e">
+      <c r="K134" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" s="37" t="n">
         <f aca="false">J134-K134-L134</f>
-        <v>#REF!</v>
+        <v>13000</v>
       </c>
       <c r="N134" s="78" t="s">
         <v>375</v>
@@ -8371,14 +8408,15 @@
         <f aca="false">13000</f>
         <v>13000</v>
       </c>
-      <c r="K135" s="36" t="e">
-        <f aca="false">#REF!*I135*J135</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L135" s="36"/>
-      <c r="M135" s="37" t="e">
+      <c r="K135" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" s="37" t="n">
         <f aca="false">J135-K135-L135</f>
-        <v>#REF!</v>
+        <v>13000</v>
       </c>
       <c r="N135" s="78" t="s">
         <v>375</v>
@@ -8413,14 +8451,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K136" s="36" t="e">
-        <f aca="false">#REF!*I136*J136</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L136" s="36"/>
-      <c r="M136" s="37" t="e">
+      <c r="K136" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" s="37" t="n">
         <f aca="false">J136-K136-L136</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N136" s="78" t="s">
         <v>375</v>
@@ -8455,14 +8494,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K137" s="36" t="e">
-        <f aca="false">#REF!*I137*J137</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L137" s="36"/>
-      <c r="M137" s="37" t="e">
+      <c r="K137" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" s="37" t="n">
         <f aca="false">J137-K137-L137</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N137" s="78" t="s">
         <v>375</v>
@@ -8497,14 +8537,15 @@
         <f aca="false">8500</f>
         <v>8500</v>
       </c>
-      <c r="K138" s="36" t="e">
-        <f aca="false">#REF!*I138*J138</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L138" s="36"/>
-      <c r="M138" s="37" t="e">
+      <c r="K138" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M138" s="37" t="n">
         <f aca="false">J138-K138-L138</f>
-        <v>#REF!</v>
+        <v>8500</v>
       </c>
       <c r="N138" s="78" t="s">
         <v>375</v>
@@ -8538,14 +8579,15 @@
       <c r="J139" s="81" t="n">
         <v>8000</v>
       </c>
-      <c r="K139" s="36" t="e">
-        <f aca="false">#REF!*I139*J139</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L139" s="36"/>
-      <c r="M139" s="37" t="e">
+      <c r="K139" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" s="37" t="n">
         <f aca="false">J139-K139-L139</f>
-        <v>#REF!</v>
+        <v>8000</v>
       </c>
       <c r="N139" s="78" t="s">
         <v>375</v>
@@ -8580,14 +8622,15 @@
         <f aca="false">8000</f>
         <v>8000</v>
       </c>
-      <c r="K140" s="36" t="e">
-        <f aca="false">#REF!*I140*J140</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L140" s="36"/>
-      <c r="M140" s="37" t="e">
+      <c r="K140" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" s="37" t="n">
         <f aca="false">J140-K140-L140</f>
-        <v>#REF!</v>
+        <v>8000</v>
       </c>
       <c r="N140" s="78" t="s">
         <v>375</v>
@@ -8621,14 +8664,15 @@
       <c r="J141" s="81" t="n">
         <v>7000</v>
       </c>
-      <c r="K141" s="36" t="e">
-        <f aca="false">#REF!*I141*J141</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L141" s="36"/>
-      <c r="M141" s="37" t="e">
+      <c r="K141" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" s="37" t="n">
         <f aca="false">J141-K141-L141</f>
-        <v>#REF!</v>
+        <v>7000</v>
       </c>
       <c r="N141" s="78" t="s">
         <v>375</v>
@@ -8663,14 +8707,15 @@
         <f aca="false">31304.35</f>
         <v>31304.35</v>
       </c>
-      <c r="K142" s="36" t="e">
-        <f aca="false">#REF!*I142*J142</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L142" s="36"/>
-      <c r="M142" s="37" t="e">
+      <c r="K142" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" s="37" t="n">
         <f aca="false">J142-K142-L142</f>
-        <v>#REF!</v>
+        <v>31304.35</v>
       </c>
       <c r="N142" s="78" t="s">
         <v>375</v>
@@ -8705,14 +8750,15 @@
         <f aca="false">31304.35</f>
         <v>31304.35</v>
       </c>
-      <c r="K143" s="36" t="e">
-        <f aca="false">#REF!*I143*J143</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L143" s="36"/>
-      <c r="M143" s="37" t="e">
+      <c r="K143" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" s="37" t="n">
         <f aca="false">J143-K143-L143</f>
-        <v>#REF!</v>
+        <v>31304.35</v>
       </c>
       <c r="N143" s="78" t="s">
         <v>375</v>
@@ -8721,7 +8767,7 @@
       <c r="P143" s="26"/>
       <c r="AMJ143" s="0"/>
     </row>
-    <row r="144" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="42" t="n">
         <v>42637</v>
       </c>
@@ -8770,7 +8816,7 @@
       <c r="P144" s="26"/>
       <c r="AMJ144" s="0"/>
     </row>
-    <row r="145" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="42" t="n">
         <v>40493</v>
       </c>
@@ -9159,7 +9205,7 @@
       <c r="P152" s="26"/>
       <c r="AMJ152" s="0"/>
     </row>
-    <row r="153" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="44" t="n">
         <f aca="false">A39</f>
         <v>42878</v>
@@ -9173,7 +9219,7 @@
       </c>
       <c r="D153" s="85" t="str">
         <f aca="false">D39</f>
-        <v>Jupiter Trading </v>
+        <v>Jupiter Trading</v>
       </c>
       <c r="E153" s="86" t="str">
         <f aca="false">E39</f>
@@ -9213,7 +9259,7 @@
       <c r="P153" s="26"/>
       <c r="AMJ153" s="0"/>
     </row>
-    <row r="154" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="28" t="n">
         <f aca="false">A39</f>
         <v>42878</v>
@@ -9318,7 +9364,7 @@
       <c r="P155" s="26"/>
       <c r="AMJ155" s="0"/>
     </row>
-    <row r="156" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="18" t="n">
         <v>42838</v>
       </c>
@@ -9363,7 +9409,7 @@
       <c r="P156" s="26"/>
       <c r="AMJ156" s="0"/>
     </row>
-    <row r="157" s="27" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" s="27" customFormat="true" ht="33.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="44" t="n">
         <v>41338</v>
       </c>
@@ -9384,7 +9430,7 @@
       <c r="J157" s="35" t="n">
         <v>2350</v>
       </c>
-      <c r="K157" s="36" t="n">
+      <c r="K157" s="37" t="n">
         <v>0</v>
       </c>
       <c r="L157" s="37" t="n">

</xml_diff>